<commit_message>
Add responsible Person to Data Source -> v0.2.0
</commit_message>
<xml_diff>
--- a/data/example/Data_Sources.xlsx
+++ b/data/example/Data_Sources.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataSources" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DataSources" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -521,13 +521,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
@@ -544,7 +544,8 @@
     <col width="28.7109375" customWidth="1" min="4" max="4"/>
     <col width="20.7109375" customWidth="1" min="5" max="5"/>
     <col width="25.7109375" customWidth="1" min="6" max="6"/>
-    <col width="100.7109375" customWidth="1" min="7" max="7"/>
+    <col width="25.7109375" customWidth="1" min="7" max="7"/>
+    <col width="100.7109375" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -559,6 +560,7 @@
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="3" t="inlineStr">
@@ -568,7 +570,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.0</t>
+          <t>v0.2.0</t>
         </is>
       </c>
     </row>
@@ -595,10 +597,15 @@
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
+          <t>Person Responsible</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
           <t>Date Last Edited</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="H3" s="5" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
@@ -627,10 +634,15 @@
       </c>
       <c r="F4" s="6" t="inlineStr">
         <is>
+          <t>personResponsible</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr">
+        <is>
           <t>lastEdited</t>
         </is>
       </c>
-      <c r="G4" s="6" t="inlineStr">
+      <c r="H4" s="6" t="inlineStr">
         <is>
           <t>comments</t>
         </is>
@@ -659,10 +671,15 @@
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
+          <t>Person responsible that added this source and the corresponding entries</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
           <t>Date of last edit (most likely when it was created)</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr">
+      <c r="H5" s="7" t="inlineStr">
         <is>
           <t>Additional comments, manual adjustments, etc.</t>
         </is>
@@ -699,6 +716,11 @@
           <t>-</t>
         </is>
       </c>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="9" t="inlineStr">
@@ -723,10 +745,15 @@
       </c>
       <c r="F7" s="9" t="inlineStr">
         <is>
+          <t>[text]</t>
+        </is>
+      </c>
+      <c r="G7" s="9" t="inlineStr">
+        <is>
           <t>[date]</t>
         </is>
       </c>
-      <c r="G7" s="9" t="inlineStr">
+      <c r="H7" s="9" t="inlineStr">
         <is>
           <t>[text]</t>
         </is>
@@ -753,10 +780,15 @@
       </c>
       <c r="F8" s="11" t="inlineStr">
         <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="G8" s="11" t="inlineStr">
+        <is>
           <t>30.01.2025</t>
         </is>
       </c>
-      <c r="G8" s="11" t="inlineStr">
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>No manual adjustment</t>
         </is>
@@ -783,10 +815,15 @@
       </c>
       <c r="F9" s="11" t="inlineStr">
         <is>
+          <t>Tester</t>
+        </is>
+      </c>
+      <c r="G9" s="11" t="inlineStr">
+        <is>
           <t>30.01.2025</t>
         </is>
       </c>
-      <c r="G9" s="11" t="inlineStr">
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>Resistances adj. by factor 2.1 (not really, comment is just for testing)</t>
         </is>
@@ -794,6 +831,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>